<commit_message>
1. Main-2.2.py: update water intervals and time format in log files. 2. Add Trials without video
</commit_message>
<xml_diff>
--- a/Expense.xlsx
+++ b/Expense.xlsx
@@ -434,7 +434,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -479,8 +479,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -568,7 +572,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
+      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1384,8 +1388,7 @@
         <v>6.26</v>
       </c>
       <c r="E32" s="11" t="n">
-        <f aca="false">SUM(D32:D39)</f>
-        <v>250.14</v>
+        <v>224.63</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>10</v>
@@ -1515,10 +1518,10 @@
       <c r="F37" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G37" s="0" t="s">
+      <c r="G37" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H37" s="12" t="s">
+      <c r="H37" s="13" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1579,7 +1582,7 @@
       </c>
       <c r="E41" s="1" t="n">
         <f aca="false">1000-SUM(E2:E40)</f>
-        <v>169.32</v>
+        <v>194.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20210621 meeting and purchase
</commit_message>
<xml_diff>
--- a/Expense.xlsx
+++ b/Expense.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="122">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -323,6 +323,66 @@
   </si>
   <si>
     <t xml:space="preserve">https://uk.rs-online.com/web/p/heat-shrink-cold-shrink-sleeves/9146802/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandisk Micro SD Card 128 GB MicroSDXC Card Class 10, UHS-1 U1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">174-7340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://uk.rs-online.com/web/p/micro-sd-cards/1747340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS PRO RS41 K Input Wired Digital Thermometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123-1940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://uk.rs-online.com/web/p/products/1231940/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS PRO Digital Timer Switch 230 V ac 100h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">178-5368</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://uk.rs-online.com/web/p/time-switches/1785368/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS PRO, 24 V dc, DC Axial Fan, 80 x 80 x 25mm, 68m³/h, 2.4W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">668-8833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://uk.rs-online.com/web/p/axial-fans/6688833/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fan Filter, Fan Mounted 86.5 x 86.5mm, for 80mm Fan PET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">221-336</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://uk.rs-online.com/web/p/fan-filters/0221336/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS PRO, 20W Plug In Power Supply 24V ac, 800mA Type G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">139-1777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://uk.rs-online.com/web/p/ac-dc-adapters/1391777/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seeed Studio, SPDT Relay – 103020133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brennenstuhl 3m 6 Socket Type G - British Extension Lead, 230 V </t>
   </si>
   <si>
     <t xml:space="preserve">Remain</t>
@@ -338,7 +398,7 @@
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -388,6 +448,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -434,7 +499,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -479,15 +544,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -569,10 +638,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1387,7 +1456,7 @@
         <f aca="false">B32*C32</f>
         <v>6.26</v>
       </c>
-      <c r="E32" s="11" t="n">
+      <c r="E32" s="3" t="n">
         <v>224.63</v>
       </c>
       <c r="F32" s="4" t="s">
@@ -1414,7 +1483,7 @@
         <f aca="false">B33*C33</f>
         <v>19.55</v>
       </c>
-      <c r="E33" s="11"/>
+      <c r="E33" s="3"/>
       <c r="F33" s="4" t="s">
         <v>10</v>
       </c>
@@ -1439,7 +1508,7 @@
         <f aca="false">B34*C34</f>
         <v>29.17</v>
       </c>
-      <c r="E34" s="11"/>
+      <c r="E34" s="3"/>
       <c r="F34" s="4" t="s">
         <v>10</v>
       </c>
@@ -1464,7 +1533,7 @@
         <f aca="false">B35*C35</f>
         <v>22.21</v>
       </c>
-      <c r="E35" s="11"/>
+      <c r="E35" s="3"/>
       <c r="F35" s="4" t="s">
         <v>10</v>
       </c>
@@ -1489,7 +1558,7 @@
         <f aca="false">B36*C36</f>
         <v>145.6</v>
       </c>
-      <c r="E36" s="11"/>
+      <c r="E36" s="3"/>
       <c r="F36" s="4" t="s">
         <v>10</v>
       </c>
@@ -1514,14 +1583,14 @@
         <f aca="false">B37*C37</f>
         <v>6.1</v>
       </c>
-      <c r="E37" s="11"/>
+      <c r="E37" s="3"/>
       <c r="F37" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G37" s="12" t="s">
+      <c r="G37" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="H37" s="12" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1539,7 +1608,7 @@
         <f aca="false">B38*C38</f>
         <v>16.8</v>
       </c>
-      <c r="E38" s="11"/>
+      <c r="E38" s="3"/>
       <c r="F38" s="4" t="s">
         <v>10</v>
       </c>
@@ -1564,7 +1633,7 @@
         <f aca="false">B39*C39</f>
         <v>4.45</v>
       </c>
-      <c r="E39" s="11"/>
+      <c r="E39" s="3"/>
       <c r="F39" s="4" t="s">
         <v>10</v>
       </c>
@@ -1576,21 +1645,251 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E41" s="1" t="n">
-        <f aca="false">1000-SUM(E2:E40)</f>
-        <v>194.83</v>
+      <c r="B41" s="1" t="n">
+        <v>69.34</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <f aca="false">B41*C41</f>
+        <v>69.34</v>
+      </c>
+      <c r="E41" s="13" t="n">
+        <f aca="false">181.53*1.2</f>
+        <v>217.836</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>47.18</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <f aca="false">B42*C42</f>
+        <v>47.18</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="F42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>18.56</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <f aca="false">B43*C43</f>
+        <v>18.56</v>
+      </c>
+      <c r="E43" s="13"/>
+      <c r="F43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>9.72</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <f aca="false">B44*C44</f>
+        <v>9.72</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>5.82</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <f aca="false">B45*C45</f>
+        <v>5.82</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>11.89</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <f aca="false">B46*C46</f>
+        <v>11.89</v>
+      </c>
+      <c r="E46" s="13"/>
+      <c r="F46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>29.17</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1" t="n">
+        <f aca="false">B47*C47</f>
+        <v>29.17</v>
+      </c>
+      <c r="E47" s="13"/>
+      <c r="F47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>9.06</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <f aca="false">B48*C48</f>
+        <v>9.06</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="F48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" s="1" t="n">
+        <v>19.55</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <f aca="false">B49*C49</f>
+        <v>19.55</v>
+      </c>
+      <c r="E49" s="13"/>
+      <c r="F49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E51" s="1" t="n">
+        <f aca="false">3000-SUM(E2:E50)</f>
+        <v>1976.994</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="E2:E9"/>
     <mergeCell ref="E11:E19"/>
     <mergeCell ref="E23:E30"/>
     <mergeCell ref="E32:E39"/>
+    <mergeCell ref="E41:E49"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H21" r:id="rId1" display="https://uk.rs-online.com/web/p/raspberry-pi-os/1213897/"/>
@@ -1610,6 +1909,15 @@
     <hyperlink ref="H37" r:id="rId15" display="https://uk.rs-online.com/web/p/mains-plugs-sockets/0854380/"/>
     <hyperlink ref="H38" r:id="rId16" display="https://uk.rs-online.com/web/p/standard-terminal-blocks/7822857?cm_mmc=UK-PLA-DS3A-_-google-_-CSS_UK_EN_Connectors_Whoop-_-Standard+Terminal+Blocks_Whoop+(2)-_-7822857&amp;matchtype=&amp;aud-826607888547:pla-302090786601&amp;gclid=Cj0KCQjwyZmEBhCpARIsALIzmnLCHxAQ4jYSvQ67LUSVpl-s1F3SjJgTcXCgc59uX36_UIUZsUNBkCMaAnZYEALw_wcB&amp;gclsrc=aw.ds"/>
     <hyperlink ref="H39" r:id="rId17" display="https://uk.rs-online.com/web/p/heat-shrink-cold-shrink-sleeves/9146802/"/>
+    <hyperlink ref="H41" r:id="rId18" display="https://uk.rs-online.com/web/p/micro-sd-cards/1747340"/>
+    <hyperlink ref="H42" r:id="rId19" display="https://uk.rs-online.com/web/p/products/1231940/"/>
+    <hyperlink ref="H43" r:id="rId20" display="https://uk.rs-online.com/web/p/time-switches/1785368/"/>
+    <hyperlink ref="H44" r:id="rId21" display="https://uk.rs-online.com/web/p/axial-fans/6688833/"/>
+    <hyperlink ref="H45" r:id="rId22" display="https://uk.rs-online.com/web/p/fan-filters/0221336/"/>
+    <hyperlink ref="H46" r:id="rId23" display="https://uk.rs-online.com/web/p/ac-dc-adapters/1391777/"/>
+    <hyperlink ref="H47" r:id="rId24" display="https://uk.rs-online.com/web/p/3d-printing-materials/8320223/"/>
+    <hyperlink ref="H48" r:id="rId25" display="https://uk.rs-online.com/web/p/power-motor-robotics-development-tools/1845099"/>
+    <hyperlink ref="H49" r:id="rId26" display="https://uk.rs-online.com/web/p/extension-leads-cable-reels/7685320/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>